<commit_message>
updated excel export of 12 min data
</commit_message>
<xml_diff>
--- a/simulated_electrolyzer_loads_12min_2019-10-02.xlsx
+++ b/simulated_electrolyzer_loads_12min_2019-10-02.xlsx
@@ -449,27 +449,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>simulated_combined_load_e1</t>
+          <t>Combined_E1_Load_kW</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>simulated_combined_load_e2</t>
+          <t>Combined_E2_Load_kW</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>simulated_combined_load_e1_ramp_type</t>
+          <t>Combined_E1_Ramp_Type</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>simulated_combined_load_e2_ramp_type</t>
+          <t>Combined_E2_Ramp_Type</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>combined_hydrogen_production</t>
+          <t>Combined_Hydrogen_Production_kg</t>
         </is>
       </c>
     </row>
@@ -2448,27 +2448,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>simulated_wind_load_e1</t>
+          <t>Wind_E1_Load_kW</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>simulated_wind_load_e2</t>
+          <t>Wind_E2_Load_kW</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>simulated_wind_load_e1_ramp_type</t>
+          <t>Wind_E1_Ramp_Type</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>simulated_wind_load_e2_ramp_type</t>
+          <t>Wind_E2_Ramp_Type</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>wind_hydrogen_production</t>
+          <t>Wind_Hydrogen_Production_kg</t>
         </is>
       </c>
     </row>
@@ -4423,27 +4423,27 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>simulated_solar_load_e1</t>
+          <t>Solar_E1_Load_kW</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>simulated_solar_load_e2</t>
+          <t>Solar_E2_Load_kW</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>simulated_solar_load_e1_ramp_type</t>
+          <t>Solar_E1_Ramp_Type</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>simulated_solar_load_e2_ramp_type</t>
+          <t>Solar_E2_Ramp_Type</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>solar_hydrogen_production</t>
+          <t>Solar_Hydrogen_Production_kg</t>
         </is>
       </c>
     </row>

</xml_diff>